<commit_message>
continued to test and develope the repeater
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/Repeater/BIIB/BIIBBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/Repeater/BIIB/BIIBBag.xlsx
@@ -527,22 +527,22 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42651.426087962966</v>
+        <v>42651.599548611113</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
       </c>
       <c r="D2">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E2">
-        <v>7919</v>
+        <v>8268</v>
       </c>
       <c r="F2">
-        <v>913</v>
+        <v>949</v>
       </c>
       <c r="G2">
         <v>60</v>
@@ -551,31 +551,31 @@
         <v>38</v>
       </c>
       <c r="I2">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="J2">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="K2">
-        <v>21457</v>
+        <v>42059</v>
       </c>
       <c r="L2">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="M2">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N2">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="O2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P2" t="s">
         <v>26</v>
       </c>
       <c r="Q2">
-        <v>44.409435964196724</v>
+        <v>46.242130528922125</v>
       </c>
       <c r="R2">
         <v>1.8</v>
@@ -593,7 +593,7 @@
         <v>27</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>